<commit_message>
updated Excel, pivot chart bar graph
</commit_message>
<xml_diff>
--- a/MachineLearningModelRatings.xlsx
+++ b/MachineLearningModelRatings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/Code/UA Bootcamp Homework/21-Machine Learning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/machine-learning-challenge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946E1CF9-1E4D-944C-923C-2990C9DB28FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{281826F0-0E3D-C54F-A79C-8C6B1577442E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2640" yWindow="460" windowWidth="23320" windowHeight="16140" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Machine Learning Model comparison for Kepler Exoplanet Data</t>
   </si>
@@ -58,12 +58,18 @@
   <si>
     <t>Rating (%)</t>
   </si>
+  <si>
+    <t>Neureal Network</t>
+  </si>
+  <si>
+    <t>kNN</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -246,9 +252,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$4:$A$8</c:f>
+              <c:f>Sheet1!$A$4:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Linear Regression</c:v>
                 </c:pt>
@@ -259,9 +265,15 @@
                   <c:v>Logistic Regression</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>kNN</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>Decsion Tree</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>Neureal Network</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Random Forest Classifier</c:v>
                 </c:pt>
               </c:strCache>
@@ -269,10 +281,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$8</c:f>
+              <c:f>Sheet1!$B$4:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>35.299999999999997</c:v>
                 </c:pt>
@@ -283,9 +295,15 @@
                   <c:v>65.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>80.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>82.3</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>82.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>87.2</c:v>
                 </c:pt>
               </c:numCache>
@@ -1344,24 +1362,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3DC1A6C-82E6-4F49-8C75-88DB229D9FBD}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1369,7 +1387,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1377,7 +1395,7 @@
         <v>35.299999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1385,7 +1403,7 @@
         <v>49.7</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1393,25 +1411,41 @@
         <v>65.8</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>80.099999999999994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>82.3</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>82.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="B8">
+      <c r="B10">
         <v>87.2</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B8">
-    <sortCondition ref="B4:B8"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B10">
+    <sortCondition ref="B4:B10"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
separated DT from RFC
</commit_message>
<xml_diff>
--- a/MachineLearningModelRatings.xlsx
+++ b/MachineLearningModelRatings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/machine-learning-challenge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{281826F0-0E3D-C54F-A79C-8C6B1577442E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76213ED-973D-B545-81A9-BFCF059F60A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2640" yWindow="460" windowWidth="23320" windowHeight="16140" xr2:uid="{313DD4AE-364D-A749-B1C5-94794B389EE3}"/>
   </bookViews>
@@ -298,7 +298,7 @@
                   <c:v>80.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>82.3</c:v>
+                  <c:v>82.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>82.4</c:v>
@@ -1365,7 +1365,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1424,7 +1424,7 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>82.3</v>
+        <v>82.2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>